<commit_message>
skonczenie pracy, dodanie opisu, efektywnosc, przyspiesznie, excel
</commit_message>
<xml_diff>
--- a/wykresy_czasowe.xlsx
+++ b/wykresy_czasowe.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sagro\Desktop\INFORMATYKA\pr4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5F683E86-4752-41C7-BA86-C43732496D7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4263C12F-37EE-4237-A349-F523748B3D3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{342B8391-8943-4581-A219-F291E965E96F}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{342B8391-8943-4581-A219-F291E965E96F}"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="12">
   <si>
     <t>n_threads</t>
   </si>
@@ -55,6 +55,24 @@
   <si>
     <t xml:space="preserve">Seq -&gt; </t>
   </si>
+  <si>
+    <t>S 10^5</t>
+  </si>
+  <si>
+    <t>S 10^6</t>
+  </si>
+  <si>
+    <t>S 10^7</t>
+  </si>
+  <si>
+    <t>E 10^5</t>
+  </si>
+  <si>
+    <t>E 10^6</t>
+  </si>
+  <si>
+    <t>E 10^7</t>
+  </si>
 </sst>
 </file>
 
@@ -70,15 +88,33 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -86,13 +122,31 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
@@ -199,33 +253,7 @@
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
-            <c:strRef>
-              <c:f>Arkusz1!$B$2:$B$8</c:f>
-              <c:strCache>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>0,01</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0,01</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0,01</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0,01</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0,01</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0,01</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0,01</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+            <c:v>wielowatkowo</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="28575" cap="rnd">
@@ -291,6 +319,9 @@
         <c:ser>
           <c:idx val="1"/>
           <c:order val="1"/>
+          <c:tx>
+            <c:v>sekwencyjnie</c:v>
+          </c:tx>
           <c:spPr>
             <a:ln w="28575" cap="rnd">
               <a:solidFill>
@@ -359,6 +390,67 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="pl-PL"/>
+                  <a:t>liczba</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="pl-PL" baseline="0"/>
+                  <a:t> wątków</a:t>
+                </a:r>
+                <a:endParaRPr lang="pl-PL"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="pl-PL"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -423,6 +515,66 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="pl-PL"/>
+                  <a:t>czas</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="pl-PL" baseline="0"/>
+                  <a:t> [s]</a:t>
+                </a:r>
+                <a:endParaRPr lang="pl-PL"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="pl-PL"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="0.000" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -466,6 +618,41 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:legendEntry>
+        <c:idx val="2"/>
+        <c:delete val="1"/>
+      </c:legendEntry>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="pl-PL"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:extLst>
@@ -598,6 +785,9 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
+          <c:tx>
+            <c:v>wielowatkowo</c:v>
+          </c:tx>
           <c:spPr>
             <a:ln w="28575" cap="rnd">
               <a:solidFill>
@@ -650,6 +840,9 @@
         <c:ser>
           <c:idx val="1"/>
           <c:order val="1"/>
+          <c:tx>
+            <c:v>sekwencyjnie</c:v>
+          </c:tx>
           <c:spPr>
             <a:ln w="28575" cap="rnd">
               <a:solidFill>
@@ -825,6 +1018,37 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="pl-PL"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:extLst>
@@ -957,6 +1181,9 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
+          <c:tx>
+            <c:v>wielowatkowo</c:v>
+          </c:tx>
           <c:spPr>
             <a:ln w="28575" cap="rnd">
               <a:solidFill>
@@ -1009,6 +1236,9 @@
         <c:ser>
           <c:idx val="1"/>
           <c:order val="1"/>
+          <c:tx>
+            <c:v>sekwencyjnie</c:v>
+          </c:tx>
           <c:spPr>
             <a:ln w="28575" cap="rnd">
               <a:solidFill>
@@ -1077,6 +1307,66 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="pl-PL"/>
+                  <a:t>liczba</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="pl-PL" baseline="0"/>
+                  <a:t> wątków</a:t>
+                </a:r>
+                <a:endParaRPr lang="pl-PL"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="pl-PL"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1141,6 +1431,61 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="pl-PL"/>
+                  <a:t>czas [s]</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="pl-PL"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="0.000" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -1184,6 +1529,37 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="pl-PL"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:extLst>
@@ -1316,6 +1692,9 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
+          <c:tx>
+            <c:v>10^5</c:v>
+          </c:tx>
           <c:spPr>
             <a:ln w="28575" cap="rnd">
               <a:solidFill>
@@ -1368,6 +1747,9 @@
         <c:ser>
           <c:idx val="1"/>
           <c:order val="1"/>
+          <c:tx>
+            <c:v>10^6</c:v>
+          </c:tx>
           <c:spPr>
             <a:ln w="28575" cap="rnd">
               <a:solidFill>
@@ -1420,6 +1802,9 @@
         <c:ser>
           <c:idx val="2"/>
           <c:order val="2"/>
+          <c:tx>
+            <c:v>10^7</c:v>
+          </c:tx>
           <c:spPr>
             <a:ln w="28575" cap="rnd">
               <a:solidFill>
@@ -1488,6 +1873,61 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="pl-PL"/>
+                  <a:t>Liczba wątków</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="pl-PL"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1552,6 +1992,61 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="pl-PL"/>
+                  <a:t>czas [s]</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="pl-PL"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="0.000" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -1595,6 +2090,37 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="pl-PL"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:extLst>
@@ -3868,15 +4394,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>228600</xdr:colOff>
+      <xdr:colOff>228599</xdr:colOff>
       <xdr:row>12</xdr:row>
-      <xdr:rowOff>157162</xdr:rowOff>
+      <xdr:rowOff>157161</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>123825</xdr:colOff>
+      <xdr:colOff>190499</xdr:colOff>
       <xdr:row>27</xdr:row>
-      <xdr:rowOff>42862</xdr:rowOff>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3949,8 +4475,8 @@
     <xdr:to>
       <xdr:col>35</xdr:col>
       <xdr:colOff>368753</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>155121</xdr:rowOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>115957</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3982,13 +4508,13 @@
       <xdr:col>36</xdr:col>
       <xdr:colOff>226867</xdr:colOff>
       <xdr:row>12</xdr:row>
-      <xdr:rowOff>20040</xdr:rowOff>
+      <xdr:rowOff>20039</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>45</xdr:col>
-      <xdr:colOff>119371</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>96240</xdr:rowOff>
+      <xdr:colOff>173935</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>105102</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4335,10 +4861,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6CF9FB7D-CC71-4DCD-A5BB-4974338ACE5B}">
-  <dimension ref="A1:H11"/>
+  <dimension ref="A1:O11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
-      <selection activeCell="AX19" sqref="AX19"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="I1" sqref="I1:O8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4347,7 +4873,7 @@
     <col min="2" max="2" width="8.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4366,8 +4892,29 @@
       <c r="F1" t="s">
         <v>1</v>
       </c>
+      <c r="I1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="M1" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="N1" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="O1" s="4" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>2</v>
       </c>
@@ -4390,8 +4937,35 @@
       <c r="H2" s="1">
         <v>0.95486599999999999</v>
       </c>
+      <c r="I2" s="2">
+        <v>2</v>
+      </c>
+      <c r="J2" s="3">
+        <f>F2/B2</f>
+        <v>0.68555240793201122</v>
+      </c>
+      <c r="K2" s="3">
+        <f t="shared" ref="K2:L2" si="0">G2/C2</f>
+        <v>0.90403876053078791</v>
+      </c>
+      <c r="L2" s="3">
+        <f t="shared" si="0"/>
+        <v>0.98073081375105664</v>
+      </c>
+      <c r="M2" s="4">
+        <f>J2/$A2</f>
+        <v>0.34277620396600561</v>
+      </c>
+      <c r="N2" s="4">
+        <f>K2/$A2</f>
+        <v>0.45201938026539396</v>
+      </c>
+      <c r="O2" s="4">
+        <f>L2/$A2</f>
+        <v>0.49036540687552832</v>
+      </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>3</v>
       </c>
@@ -4414,8 +4988,35 @@
       <c r="H3" s="1">
         <v>0.95486599999999999</v>
       </c>
+      <c r="I3" s="2">
+        <v>3</v>
+      </c>
+      <c r="J3" s="3">
+        <f t="shared" ref="J3:J8" si="1">F3/B3</f>
+        <v>0.68830516981763423</v>
+      </c>
+      <c r="K3" s="3">
+        <f t="shared" ref="K3:K8" si="2">G3/C3</f>
+        <v>0.9755745444613525</v>
+      </c>
+      <c r="L3" s="3">
+        <f t="shared" ref="L3:L8" si="3">H3/D3</f>
+        <v>1.5383968460855597</v>
+      </c>
+      <c r="M3" s="4">
+        <f>J3/$A3</f>
+        <v>0.22943505660587807</v>
+      </c>
+      <c r="N3" s="4">
+        <f>K3/$A3</f>
+        <v>0.32519151482045083</v>
+      </c>
+      <c r="O3" s="4">
+        <f>L3/$A3</f>
+        <v>0.51279894869518661</v>
+      </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>4</v>
       </c>
@@ -4438,8 +5039,35 @@
       <c r="H4" s="1">
         <v>0.95486599999999999</v>
       </c>
+      <c r="I4" s="2">
+        <v>4</v>
+      </c>
+      <c r="J4" s="3">
+        <f t="shared" si="1"/>
+        <v>0.39930117441521884</v>
+      </c>
+      <c r="K4" s="3">
+        <f t="shared" si="2"/>
+        <v>0.70394301561158268</v>
+      </c>
+      <c r="L4" s="3">
+        <f t="shared" si="3"/>
+        <v>1.4092590242131393</v>
+      </c>
+      <c r="M4" s="4">
+        <f>J4/$A4</f>
+        <v>9.982529360380471E-2</v>
+      </c>
+      <c r="N4" s="4">
+        <f>K4/$A4</f>
+        <v>0.17598575390289567</v>
+      </c>
+      <c r="O4" s="4">
+        <f>L4/$A4</f>
+        <v>0.35231475605328483</v>
+      </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>5</v>
       </c>
@@ -4462,8 +5090,35 @@
       <c r="H5" s="1">
         <v>0.95486599999999999</v>
       </c>
+      <c r="I5" s="2">
+        <v>5</v>
+      </c>
+      <c r="J5" s="3">
+        <f t="shared" si="1"/>
+        <v>0.29777070063694266</v>
+      </c>
+      <c r="K5" s="3">
+        <f t="shared" si="2"/>
+        <v>0.61755625262429914</v>
+      </c>
+      <c r="L5" s="3">
+        <f t="shared" si="3"/>
+        <v>1.3836311576604514</v>
+      </c>
+      <c r="M5" s="4">
+        <f>J5/$A5</f>
+        <v>5.9554140127388536E-2</v>
+      </c>
+      <c r="N5" s="4">
+        <f>K5/$A5</f>
+        <v>0.12351125052485983</v>
+      </c>
+      <c r="O5" s="4">
+        <f>L5/$A5</f>
+        <v>0.27672623153209031</v>
+      </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>6</v>
       </c>
@@ -4486,8 +5141,35 @@
       <c r="H6" s="1">
         <v>0.95486599999999999</v>
       </c>
+      <c r="I6" s="2">
+        <v>6</v>
+      </c>
+      <c r="J6" s="3">
+        <f t="shared" si="1"/>
+        <v>0.46033344522770497</v>
+      </c>
+      <c r="K6" s="3">
+        <f t="shared" si="2"/>
+        <v>0.519758860825278</v>
+      </c>
+      <c r="L6" s="3">
+        <f t="shared" si="3"/>
+        <v>1.0047403039476577</v>
+      </c>
+      <c r="M6" s="4">
+        <f>J6/$A6</f>
+        <v>7.6722240871284167E-2</v>
+      </c>
+      <c r="N6" s="4">
+        <f>K6/$A6</f>
+        <v>8.6626476804212996E-2</v>
+      </c>
+      <c r="O6" s="4">
+        <f>L6/$A6</f>
+        <v>0.16745671732460962</v>
+      </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>7</v>
       </c>
@@ -4510,8 +5192,35 @@
       <c r="H7" s="1">
         <v>0.95486599999999999</v>
       </c>
+      <c r="I7" s="2">
+        <v>7</v>
+      </c>
+      <c r="J7" s="3">
+        <f t="shared" si="1"/>
+        <v>0.43392047252399535</v>
+      </c>
+      <c r="K7" s="3">
+        <f t="shared" si="2"/>
+        <v>0.52231587963108028</v>
+      </c>
+      <c r="L7" s="3">
+        <f t="shared" si="3"/>
+        <v>1.0377929187592994</v>
+      </c>
+      <c r="M7" s="4">
+        <f>J7/$A7</f>
+        <v>6.1988638931999338E-2</v>
+      </c>
+      <c r="N7" s="4">
+        <f>K7/$A7</f>
+        <v>7.4616554233011473E-2</v>
+      </c>
+      <c r="O7" s="4">
+        <f>L7/$A7</f>
+        <v>0.14825613125132847</v>
+      </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>8</v>
       </c>
@@ -4534,11 +5243,41 @@
       <c r="H8" s="1">
         <v>0.95486599999999999</v>
       </c>
+      <c r="I8" s="2">
+        <v>8</v>
+      </c>
+      <c r="J8" s="3">
+        <f t="shared" si="1"/>
+        <v>0.31795347399335339</v>
+      </c>
+      <c r="K8" s="3">
+        <f t="shared" si="2"/>
+        <v>0.46947378303525328</v>
+      </c>
+      <c r="L8" s="3">
+        <f t="shared" si="3"/>
+        <v>0.9409039266326974</v>
+      </c>
+      <c r="M8" s="4">
+        <f>J8/$A8</f>
+        <v>3.9744184249169173E-2</v>
+      </c>
+      <c r="N8" s="4">
+        <f>K8/$A8</f>
+        <v>5.868422287940666E-2</v>
+      </c>
+      <c r="O8" s="4">
+        <f>L8/$A8</f>
+        <v>0.11761299082908717</v>
+      </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>4</v>
       </c>
+      <c r="B10" t="s">
+        <v>1</v>
+      </c>
       <c r="C10" t="s">
         <v>2</v>
       </c>
@@ -4546,7 +5285,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>1</v>
       </c>

</xml_diff>